<commit_message>
add additional dummy data
</commit_message>
<xml_diff>
--- a/data/attendance.xlsx
+++ b/data/attendance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\initi\Development\ranking\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FFA6DEC-DEFB-44BB-B3E6-1211745EF2BD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C0DA546-8699-4CF4-896B-3F90AC135CA8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{7D251358-1EA4-494F-9A13-C83C3F088627}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>File Number</t>
   </si>
@@ -85,6 +85,36 @@
   </si>
   <si>
     <t>Points</t>
+  </si>
+  <si>
+    <t>SCOTT, Michael</t>
+  </si>
+  <si>
+    <t>BERTRAM, Nellie</t>
+  </si>
+  <si>
+    <t>CALIFORNIA, Robert</t>
+  </si>
+  <si>
+    <t>LEVINSON, Jan</t>
+  </si>
+  <si>
+    <t>MILLER, Pete</t>
+  </si>
+  <si>
+    <t>ANDERSON, Roy</t>
+  </si>
+  <si>
+    <t>MINER, Charles</t>
+  </si>
+  <si>
+    <t>BENNETT, Jo</t>
+  </si>
+  <si>
+    <t>GREEN, Clark</t>
+  </si>
+  <si>
+    <t>VANCE, Bob</t>
   </si>
 </sst>
 </file>
@@ -93,7 +123,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -128,7 +158,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26B62ECF-5D47-43D0-9324-9B819C13405B}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="A28" sqref="A28:XFD28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -671,6 +701,126 @@
       </c>
       <c r="D18" s="1"/>
     </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>123473</v>
+      </c>
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="1">
+        <v>7</v>
+      </c>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>123474</v>
+      </c>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="1">
+        <v>6</v>
+      </c>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>123475</v>
+      </c>
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>123476</v>
+      </c>
+      <c r="B22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="1">
+        <v>8</v>
+      </c>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>123477</v>
+      </c>
+      <c r="B23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="1">
+        <v>6.5</v>
+      </c>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>123478</v>
+      </c>
+      <c r="B24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="1">
+        <v>9</v>
+      </c>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>123479</v>
+      </c>
+      <c r="B25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="1">
+        <v>4</v>
+      </c>
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>123480</v>
+      </c>
+      <c r="B26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" s="1">
+        <v>0</v>
+      </c>
+      <c r="D26" s="1"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>123481</v>
+      </c>
+      <c r="B27" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" s="1">
+        <v>6</v>
+      </c>
+      <c r="D27" s="1"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>123483</v>
+      </c>
+      <c r="B28" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" s="1">
+        <v>8</v>
+      </c>
+      <c r="D28" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>